<commit_message>
working on how to identify a mooring line or not
</commit_message>
<xml_diff>
--- a/main/other/CHAT3-4.xlsx
+++ b/main/other/CHAT3-4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\main\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1822BB-DD4E-468D-8AC5-23DF29E091AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B47138-24A6-4B0D-8D0C-18B9CBD5B237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2220" windowWidth="9720" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1302,8 +1302,8 @@
   </sheetPr>
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1403,11 +1403,11 @@
         <v>-83.3</v>
       </c>
       <c r="D7" s="27">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E7" s="28">
         <f>SUM(D7:D58 )</f>
-        <v>147.04860000000002</v>
+        <v>146.54860000000002</v>
       </c>
       <c r="F7" s="27">
         <f>SUM(C10:C55)</f>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="G7" s="29">
         <f>A2-E7</f>
-        <v>12.951399999999978</v>
+        <v>13.451399999999978</v>
       </c>
       <c r="H7" s="93"/>
     </row>

</xml_diff>